<commit_message>
Mise à jour du 01/06/25
</commit_message>
<xml_diff>
--- a/CAN 2025/Résultats CAN 2025.xlsx
+++ b/CAN 2025/Résultats CAN 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gaelle\work-linux\cours-2024-2025\CAN 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gaelle\work-linux\cours24-25\CAN 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FE2C0E-CAC9-4759-9383-4A7737F285EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC21995-1365-4979-B640-BEADCF4B2C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{16B938D3-D974-42AE-AF53-A29C2918EBD1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{16B938D3-D974-42AE-AF53-A29C2918EBD1}"/>
   </bookViews>
   <sheets>
     <sheet name="TCo" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>23 élèves</t>
   </si>
@@ -301,37 +301,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -674,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8615CFE-1476-4947-BDFF-7E2A8CEB57E7}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,13 +930,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
-      <formula>18</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C4:C26">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -978,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770EA551-9726-42AC-A79F-31DD9AEB80F6}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,6 +1197,9 @@
       <c r="B24" t="s">
         <v>43</v>
       </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1340,11 +1308,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C33">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>17</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>17</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>